<commit_message>
Worked on more compression, not good!
</commit_message>
<xml_diff>
--- a/test/vorlage.xlsx
+++ b/test/vorlage.xlsx
@@ -109,9 +109,8 @@
           <c:spPr>
             <a:ln w="25400" cap="rnd">
               <a:solidFill>
-                <a:schemeClr val="accent3">
-                  <a:lumMod val="60000"/>
-                  <a:lumOff val="40000"/>
+                <a:schemeClr val="accent2">
+                  <a:lumMod val="75000"/>
                 </a:schemeClr>
               </a:solidFill>
               <a:round/>
@@ -123,14 +122,14 @@
             <c:size val="5"/>
             <c:spPr>
               <a:solidFill>
-                <a:schemeClr val="accent3">
-                  <a:lumMod val="75000"/>
+                <a:schemeClr val="accent2">
+                  <a:lumMod val="50000"/>
                 </a:schemeClr>
               </a:solidFill>
               <a:ln w="9525">
                 <a:solidFill>
-                  <a:schemeClr val="accent3">
-                    <a:lumMod val="75000"/>
+                  <a:schemeClr val="accent2">
+                    <a:lumMod val="50000"/>
                   </a:schemeClr>
                 </a:solidFill>
               </a:ln>
@@ -184,9 +183,8 @@
           <c:spPr>
             <a:ln w="25400" cap="rnd">
               <a:solidFill>
-                <a:schemeClr val="accent3">
-                  <a:lumMod val="60000"/>
-                  <a:lumOff val="40000"/>
+                <a:schemeClr val="accent2">
+                  <a:lumMod val="75000"/>
                 </a:schemeClr>
               </a:solidFill>
               <a:round/>
@@ -198,14 +196,14 @@
             <c:size val="5"/>
             <c:spPr>
               <a:solidFill>
-                <a:schemeClr val="accent3">
-                  <a:lumMod val="75000"/>
+                <a:schemeClr val="accent2">
+                  <a:lumMod val="50000"/>
                 </a:schemeClr>
               </a:solidFill>
               <a:ln w="9525">
                 <a:solidFill>
-                  <a:schemeClr val="accent3">
-                    <a:lumMod val="75000"/>
+                  <a:schemeClr val="accent2">
+                    <a:lumMod val="50000"/>
                   </a:schemeClr>
                 </a:solidFill>
               </a:ln>
@@ -259,7 +257,7 @@
           <c:spPr>
             <a:ln w="19050" cap="rnd">
               <a:solidFill>
-                <a:schemeClr val="accent2">
+                <a:schemeClr val="accent3">
                   <a:lumMod val="75000"/>
                 </a:schemeClr>
               </a:solidFill>
@@ -312,7 +310,9 @@
           <c:spPr>
             <a:ln w="19050" cap="rnd">
               <a:solidFill>
-                <a:schemeClr val="accent4"/>
+                <a:schemeClr val="accent3">
+                  <a:lumMod val="75000"/>
+                </a:schemeClr>
               </a:solidFill>
               <a:round/>
             </a:ln>
@@ -330,7 +330,7 @@
             <c:spPr>
               <a:ln w="19050" cap="rnd">
                 <a:solidFill>
-                  <a:schemeClr val="accent2">
+                  <a:schemeClr val="accent3">
                     <a:lumMod val="75000"/>
                   </a:schemeClr>
                 </a:solidFill>
@@ -381,7 +381,7 @@
           <c:spPr>
             <a:ln w="19050" cap="rnd">
               <a:solidFill>
-                <a:schemeClr val="accent2">
+                <a:schemeClr val="accent3">
                   <a:lumMod val="75000"/>
                 </a:schemeClr>
               </a:solidFill>
@@ -583,11 +583,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="382349712"/>
-        <c:axId val="382351672"/>
+        <c:axId val="307743792"/>
+        <c:axId val="307744184"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="382349712"/>
+        <c:axId val="307743792"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -700,12 +700,12 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="382351672"/>
+        <c:crossAx val="307744184"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="382351672"/>
+        <c:axId val="307744184"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -818,7 +818,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="382349712"/>
+        <c:crossAx val="307743792"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:dispUnits>
@@ -1825,7 +1825,7 @@
   <dimension ref="A1:T4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q18" sqref="Q18"/>
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
big commit, did many tests
</commit_message>
<xml_diff>
--- a/test/vorlage.xlsx
+++ b/test/vorlage.xlsx
@@ -302,7 +302,10 @@
               </a:solidFill>
               <a:ln w="25400" cap="sq">
                 <a:solidFill>
-                  <a:schemeClr val="accent4"/>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="85000"/>
+                    <a:lumOff val="15000"/>
+                  </a:schemeClr>
                 </a:solidFill>
               </a:ln>
               <a:effectLst/>
@@ -349,24 +352,30 @@
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:ln w="19050" cap="rnd">
+            <a:ln w="22225" cap="rnd">
               <a:solidFill>
-                <a:schemeClr val="accent3"/>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="85000"/>
+                  <a:lumOff val="15000"/>
+                </a:schemeClr>
               </a:solidFill>
               <a:round/>
             </a:ln>
             <a:effectLst/>
           </c:spPr>
           <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="5"/>
+            <c:symbol val="square"/>
+            <c:size val="10"/>
             <c:spPr>
               <a:solidFill>
                 <a:schemeClr val="accent3"/>
               </a:solidFill>
               <a:ln w="9525">
                 <a:solidFill>
-                  <a:schemeClr val="accent3"/>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="85000"/>
+                    <a:lumOff val="15000"/>
+                  </a:schemeClr>
                 </a:solidFill>
               </a:ln>
               <a:effectLst/>
@@ -406,11 +415,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="248917016"/>
-        <c:axId val="248915448"/>
+        <c:axId val="242571008"/>
+        <c:axId val="242572576"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="248917016"/>
+        <c:axId val="242571008"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -437,7 +446,7 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:defRPr sz="1800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
                       <a:schemeClr val="tx1">
                         <a:lumMod val="65000"/>
@@ -450,16 +459,16 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="de-CH"/>
+                  <a:rPr lang="de-CH" sz="1800"/>
                   <a:t>Median </a:t>
                 </a:r>
               </a:p>
               <a:p>
                 <a:pPr>
-                  <a:defRPr/>
+                  <a:defRPr sz="1800"/>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="de-CH"/>
+                  <a:rPr lang="de-CH" sz="1800"/>
                   <a:t>Bytes pro Feldlinie</a:t>
                 </a:r>
               </a:p>
@@ -479,7 +488,7 @@
             <a:lstStyle/>
             <a:p>
               <a:pPr>
-                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:defRPr sz="1800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                   <a:solidFill>
                     <a:schemeClr val="tx1">
                       <a:lumMod val="65000"/>
@@ -517,7 +526,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="1600" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -532,12 +541,12 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="248915448"/>
+        <c:crossAx val="242572576"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="248915448"/>
+        <c:axId val="242572576"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -564,7 +573,7 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:defRPr sz="1800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
                       <a:schemeClr val="tx1">
                         <a:lumMod val="65000"/>
@@ -577,7 +586,7 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="de-CH"/>
+                  <a:rPr lang="de-CH" sz="1800"/>
                   <a:t>Standardabweichung (Meter)</a:t>
                 </a:r>
               </a:p>
@@ -597,7 +606,7 @@
             <a:lstStyle/>
             <a:p>
               <a:pPr>
-                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:defRPr sz="1800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                   <a:solidFill>
                     <a:schemeClr val="tx1">
                       <a:lumMod val="65000"/>
@@ -635,7 +644,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="1600" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -650,9 +659,42 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="248917016"/>
+        <c:crossAx val="242571008"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
+        <c:dispUnits>
+          <c:builtInUnit val="thousands"/>
+          <c:dispUnitsLbl>
+            <c:layout/>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="de-DE"/>
+              </a:p>
+            </c:txPr>
+          </c:dispUnitsLbl>
+        </c:dispUnits>
       </c:valAx>
       <c:spPr>
         <a:noFill/>
@@ -678,7 +720,7 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr>
-            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+            <a:defRPr sz="1800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
               <a:solidFill>
                 <a:schemeClr val="tx1">
                   <a:lumMod val="65000"/>
@@ -1291,16 +1333,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>1333500</xdr:colOff>
-      <xdr:row>9</xdr:row>
-      <xdr:rowOff>19050</xdr:rowOff>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>185056</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>160564</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>18</xdr:col>
-      <xdr:colOff>171450</xdr:colOff>
-      <xdr:row>36</xdr:row>
-      <xdr:rowOff>76200</xdr:rowOff>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>555171</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>119743</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1611,8 +1653,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O5"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C4" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+    <sheetView tabSelected="1" topLeftCell="B3" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C37" sqref="C37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
ok, in the bad
</commit_message>
<xml_diff>
--- a/test/vorlage.xlsx
+++ b/test/vorlage.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -415,12 +415,13 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="304967336"/>
-        <c:axId val="250477712"/>
+        <c:axId val="228079296"/>
+        <c:axId val="228078904"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="304967336"/>
+        <c:axId val="228079296"/>
         <c:scaling>
+          <c:logBase val="10"/>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
@@ -541,12 +542,12 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="250477712"/>
+        <c:crossAx val="228078904"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="250477712"/>
+        <c:axId val="228078904"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -659,7 +660,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="304967336"/>
+        <c:crossAx val="228079296"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:dispUnits>
@@ -1653,23 +1654,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O5"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C7" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="21" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="23.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.6640625" customWidth="1"/>
+    <col min="2" max="2" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="23.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.7109375" customWidth="1"/>
     <col min="5" max="5" width="11" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="29.5546875" customWidth="1"/>
-    <col min="9" max="9" width="16.109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="29.5703125" customWidth="1"/>
+    <col min="9" max="9" width="16.140625" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>6</v>
       </c>
@@ -1689,7 +1690,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -1715,7 +1716,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>50</v>
       </c>
@@ -1755,7 +1756,7 @@
         <v>858.70933333333301</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>110</v>
       </c>
@@ -1790,7 +1791,7 @@
         <v>30014198.854871798</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>120</v>
       </c>

</xml_diff>